<commit_message>
Add :Actualizacion ieee930 diccionario de datos
</commit_message>
<xml_diff>
--- a/2.Analisis/Diccionario de datos/Diccionario_de_datos.xlsx
+++ b/2.Analisis/Diccionario de datos/Diccionario_de_datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F\Desktop\QrLean\2.Analisis\Diccionario de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABF9019-BC52-4897-B739-B527718A6C45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE6C123-4D88-4817-B009-AC6C61C57D8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="20610" windowHeight="10980" xr2:uid="{CC332E7A-07EB-43CF-973F-72FC05A6A900}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="103">
   <si>
     <t>Nombre del campo</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Tamaño</t>
   </si>
   <si>
-    <t>Null</t>
-  </si>
-  <si>
     <t>Llave primaria</t>
   </si>
   <si>
@@ -322,13 +319,37 @@
   </si>
   <si>
     <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Tipo_documentos</t>
+  </si>
+  <si>
+    <t>BigInt</t>
+  </si>
+  <si>
+    <t>id_estado_solicitud</t>
+  </si>
+  <si>
+    <t>Estados_solicitudes</t>
+  </si>
+  <si>
+    <t>Id_estado</t>
+  </si>
+  <si>
+    <t>id_estado</t>
+  </si>
+  <si>
+    <t>nombre_estado</t>
+  </si>
+  <si>
+    <t>Cerrada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,6 +401,13 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -473,7 +501,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -496,15 +524,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -514,15 +533,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -534,10 +544,32 @@
     <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -909,10 +941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CC20BFF-40BD-43EF-8083-6421F05BAC6F}">
-  <dimension ref="A2:XFC259"/>
+  <dimension ref="B2:O261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M70" sqref="M69:M70"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O78" sqref="O78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,47 +969,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
     </row>
     <row r="3" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="23">
+      <c r="B3" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="17">
         <f ca="1">TODAY()</f>
-        <v>44266</v>
-      </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
+        <v>44370</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
     </row>
     <row r="4" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
@@ -995,123 +1027,123 @@
       <c r="N4" s="2"/>
     </row>
     <row r="5" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="C8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="11">
+        <v>11</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" s="10"/>
+      <c r="O8" s="12">
         <v>1</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11" t="s">
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="24"/>
+      <c r="C9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="5" t="s">
+      <c r="D9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="11">
+        <v>30</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="12" t="s">
         <v>26</v>
-      </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="14">
-        <v>11</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="N8" s="13"/>
-      <c r="O8" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="12"/>
-      <c r="C9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="14">
-        <v>30</v>
-      </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="15" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
@@ -1121,92 +1153,92 @@
       <c r="O10" s="9"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="D11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="11">
+        <v>11</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="11"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N11" s="10"/>
+      <c r="O11" s="12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="24"/>
+      <c r="C12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="14">
+      <c r="D12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="11">
+        <v>30</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="24"/>
+      <c r="C13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="11">
         <v>11</v>
       </c>
-      <c r="F11" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="N11" s="13"/>
-      <c r="O11" s="15">
+      <c r="F13" s="11"/>
+      <c r="G13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="14">
-        <v>30</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="14">
-        <v>11</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="13" t="s">
+      <c r="I13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="15">
+      <c r="J13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="12">
         <v>1</v>
       </c>
     </row>
@@ -1226,61 +1258,61 @@
       <c r="O14" s="8"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="D15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="11">
+        <v>11</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="11"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N15" s="10"/>
+      <c r="O15" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="24"/>
+      <c r="C16" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="14">
-        <v>11</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="N15" s="13"/>
-      <c r="O15" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="12"/>
-      <c r="C16" s="13" t="s">
+      <c r="D16" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="11">
+        <v>20</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="14">
-        <v>20</v>
-      </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="15" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
@@ -1299,61 +1331,61 @@
       <c r="O17" s="8"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="D18" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="11">
+        <v>11</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N18" s="10"/>
+      <c r="O18" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="24"/>
+      <c r="C19" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="14">
-        <v>11</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="N18" s="13"/>
-      <c r="O18" s="15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="12"/>
-      <c r="C19" s="13" t="s">
+      <c r="D19" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="11">
+        <v>30</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="14">
-        <v>30</v>
-      </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="15" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
@@ -1373,316 +1405,316 @@
       <c r="O20" s="8"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="D21" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="11">
+        <v>11</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="11"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N21" s="10"/>
+      <c r="O21" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="24"/>
+      <c r="C22" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="14">
+      <c r="D22" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="11">
+        <v>30</v>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="24"/>
+      <c r="C23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="11">
+        <v>30</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="24"/>
+      <c r="C24" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="11">
         <v>11</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="N21" s="13"/>
-      <c r="O21" s="15">
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="12">
+        <v>1001277963</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="24"/>
+      <c r="C25" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="11">
+        <v>150</v>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="24"/>
+      <c r="C26" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="11">
+        <v>100</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="24"/>
+      <c r="C27" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="11">
+        <v>60</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="24"/>
+      <c r="C28" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" s="11">
+        <v>11</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="12">
+        <v>3193617146</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="24"/>
+      <c r="C29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="11">
+        <v>11</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="12"/>
-      <c r="C22" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="13" t="s">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="24"/>
+      <c r="C30" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="11">
+        <v>11</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="24"/>
+      <c r="C31" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="11">
+        <v>11</v>
+      </c>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="14">
-        <v>30</v>
-      </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
-      <c r="C23" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="14">
-        <v>30</v>
-      </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="12"/>
-      <c r="C24" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="14">
-        <v>11</v>
-      </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K24" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="15">
-        <v>1001277963</v>
-      </c>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
-      <c r="C25" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="14">
-        <v>150</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="12"/>
-      <c r="C26" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="14">
-        <v>100</v>
-      </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K26" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="12"/>
-      <c r="C27" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="14">
-        <v>60</v>
-      </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="M27" s="14"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="12"/>
-      <c r="C28" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="14">
-        <v>11</v>
-      </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="M28" s="14"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="15">
-        <v>3193617146</v>
-      </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="12"/>
-      <c r="C29" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="14">
-        <v>11</v>
-      </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="I29" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J29" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="12"/>
-      <c r="C30" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="14">
-        <v>11</v>
-      </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="I30" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J30" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="12"/>
-      <c r="C31" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="14">
-        <v>11</v>
-      </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H31" s="13" t="s">
+      <c r="I31" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I31" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="J31" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="15">
+      <c r="J31" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="12">
         <v>15</v>
       </c>
     </row>
@@ -1703,61 +1735,61 @@
       <c r="O32" s="8"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="D33" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="11">
+        <v>11</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="11"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N33" s="10"/>
+      <c r="O33" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B34" s="24"/>
+      <c r="C34" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="14">
-        <v>11</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="14"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="N33" s="13"/>
-      <c r="O33" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="12"/>
-      <c r="C34" s="13" t="s">
+      <c r="D34" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="11">
+        <v>100</v>
+      </c>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="12" t="s">
         <v>53</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" s="14">
-        <v>100</v>
-      </c>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="15" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
@@ -1777,66 +1809,66 @@
       <c r="O35" s="8"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="14">
+      <c r="D36" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="11">
         <v>11</v>
       </c>
-      <c r="F36" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" s="14"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="N36" s="13"/>
-      <c r="O36" s="15">
+      <c r="F36" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="11"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N36" s="10"/>
+      <c r="O36" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="18"/>
-      <c r="C37" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E37" s="14">
+      <c r="B37" s="20"/>
+      <c r="C37" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="11">
         <v>11</v>
       </c>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H37" s="13" t="s">
+      <c r="F37" s="11"/>
+      <c r="G37" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="I37" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="J37" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="15">
+      <c r="J37" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="12">
         <v>5</v>
       </c>
     </row>
@@ -1857,61 +1889,61 @@
       <c r="O38" s="8"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="D39" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="11">
+        <v>11</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="11"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N39" s="10"/>
+      <c r="O39" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" s="20"/>
+      <c r="C40" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D39" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E39" s="14">
-        <v>11</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" s="14"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="N39" s="13"/>
-      <c r="O39" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="18"/>
-      <c r="C40" s="13" t="s">
+      <c r="D40" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="11">
+        <v>100</v>
+      </c>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E40" s="14">
-        <v>100</v>
-      </c>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="15" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
@@ -1931,226 +1963,226 @@
       <c r="O41" s="8"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" s="13" t="s">
+      <c r="B42" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" s="14">
+      <c r="C42" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="11">
         <v>11</v>
       </c>
-      <c r="F42" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G42" s="14"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="N42" s="13"/>
-      <c r="O42" s="15">
+      <c r="F42" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="11"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N42" s="10"/>
+      <c r="O42" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="12"/>
-      <c r="C43" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" s="14">
+      <c r="B43" s="24"/>
+      <c r="C43" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="11">
         <v>11</v>
       </c>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H43" s="13" t="s">
+      <c r="F43" s="11"/>
+      <c r="G43" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I43" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="I43" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="J43" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="13"/>
-      <c r="O43" s="15">
+      <c r="J43" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="12"/>
-      <c r="C44" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" s="14">
+      <c r="B44" s="24"/>
+      <c r="C44" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="11">
         <v>11</v>
       </c>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H44" s="13" t="s">
+      <c r="F44" s="11"/>
+      <c r="G44" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I44" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="I44" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="J44" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="13"/>
-      <c r="O44" s="15">
+      <c r="J44" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="12">
         <v>3</v>
       </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E46" s="14">
+      <c r="D46" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" s="11">
         <v>11</v>
       </c>
-      <c r="F46" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G46" s="14"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="N46" s="13"/>
-      <c r="O46" s="15">
+      <c r="F46" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" s="11"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N46" s="10"/>
+      <c r="O46" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="19"/>
-      <c r="C47" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E47" s="14">
+      <c r="C47" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="11">
         <v>11</v>
       </c>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H47" s="13" t="s">
+      <c r="F47" s="11"/>
+      <c r="G47" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I47" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="I47" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="J47" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="13"/>
-      <c r="O47" s="15">
+      <c r="J47" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="19"/>
-      <c r="C48" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E48" s="14">
+      <c r="C48" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="11">
         <v>11</v>
       </c>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H48" s="13" t="s">
+      <c r="F48" s="11"/>
+      <c r="G48" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I48" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="I48" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="J48" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="13"/>
-      <c r="O48" s="15">
+      <c r="J48" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="10"/>
+      <c r="O48" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="18"/>
-      <c r="C49" s="13" t="s">
+      <c r="B49" s="20"/>
+      <c r="C49" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="11">
+        <v>11</v>
+      </c>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H49" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I49" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D49" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E49" s="14">
-        <v>11</v>
-      </c>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H49" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="I49" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J49" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="13"/>
-      <c r="O49" s="15">
+      <c r="J49" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="10"/>
+      <c r="O49" s="12">
         <v>1</v>
       </c>
     </row>
@@ -2171,646 +2203,718 @@
       <c r="O50" s="8"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="D51" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="11">
+        <v>11</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" s="11"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N51" s="10"/>
+      <c r="O51" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52" s="24"/>
+      <c r="C52" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D51" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E51" s="14">
+      <c r="D52" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="11">
+        <v>50</v>
+      </c>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K52" s="11"/>
+      <c r="L52" s="11"/>
+      <c r="M52" s="11"/>
+      <c r="N52" s="10"/>
+      <c r="O52" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B53" s="24"/>
+      <c r="C53" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K53" s="11"/>
+      <c r="L53" s="11"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="10"/>
+      <c r="O53" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54" s="24"/>
+      <c r="C54" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="11">
         <v>11</v>
       </c>
-      <c r="F51" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G51" s="14"/>
-      <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
-      <c r="J51" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="N51" s="13"/>
-      <c r="O51" s="15">
+      <c r="F54" s="11"/>
+      <c r="G54" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I54" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J54" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K54" s="11"/>
+      <c r="L54" s="11"/>
+      <c r="M54" s="11"/>
+      <c r="N54" s="10"/>
+      <c r="O54" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="12"/>
-      <c r="C52" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E52" s="14">
-        <v>50</v>
-      </c>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
-      <c r="J52" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="13"/>
-      <c r="O52" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="12"/>
-      <c r="C53" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="14"/>
-      <c r="N53" s="13"/>
-      <c r="O53" s="15" t="s">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B55" s="24"/>
+      <c r="C55" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" s="11">
+        <v>11</v>
+      </c>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J55" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K55" s="11"/>
+      <c r="L55" s="11"/>
+      <c r="M55" s="11"/>
+      <c r="N55" s="10"/>
+      <c r="O55" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B56" s="24"/>
+      <c r="C56" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="11">
+        <v>11</v>
+      </c>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H56" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I56" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J56" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="10"/>
+      <c r="O56" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B57" s="24"/>
+      <c r="C57" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="11">
+        <v>11</v>
+      </c>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H57" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J57" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="11"/>
+      <c r="N57" s="10"/>
+      <c r="O57" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B58" s="7"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="6"/>
+      <c r="K58" s="6"/>
+      <c r="L58" s="6"/>
+      <c r="M58" s="6"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="8"/>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B59" s="24" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="12"/>
-      <c r="C54" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E54" s="14">
+      <c r="C59" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" s="11">
         <v>11</v>
       </c>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H54" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="I54" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J54" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="13"/>
-      <c r="O54" s="15">
+      <c r="F59" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" s="11"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K59" s="11"/>
+      <c r="L59" s="11"/>
+      <c r="M59" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N59" s="10"/>
+      <c r="O59" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="12"/>
-      <c r="C55" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E55" s="14">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B60" s="24"/>
+      <c r="C60" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="11">
+        <v>30</v>
+      </c>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K60" s="11"/>
+      <c r="L60" s="11"/>
+      <c r="M60" s="11"/>
+      <c r="N60" s="10"/>
+      <c r="O60" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B61" s="24"/>
+      <c r="C61" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K61" s="11"/>
+      <c r="L61" s="11"/>
+      <c r="M61" s="11"/>
+      <c r="N61" s="10"/>
+      <c r="O61" s="14">
+        <v>43912</v>
+      </c>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B62" s="24"/>
+      <c r="C62" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
+      <c r="J62" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K62" s="11"/>
+      <c r="L62" s="11"/>
+      <c r="M62" s="11"/>
+      <c r="N62" s="10"/>
+      <c r="O62" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B63" s="24"/>
+      <c r="C63" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+      <c r="J63" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K63" s="11"/>
+      <c r="L63" s="11"/>
+      <c r="M63" s="11"/>
+      <c r="N63" s="10"/>
+      <c r="O63" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B64" s="24"/>
+      <c r="C64" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="11">
         <v>11</v>
       </c>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H55" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="I55" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J55" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="13"/>
-      <c r="O55" s="15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="12"/>
-      <c r="C56" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D56" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E56" s="14">
+      <c r="F64" s="11"/>
+      <c r="G64" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H64" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J64" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K64" s="11"/>
+      <c r="L64" s="11"/>
+      <c r="M64" s="11"/>
+      <c r="N64" s="10"/>
+      <c r="O64" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B65" s="7"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
+      <c r="N65" s="3"/>
+      <c r="O65" s="8"/>
+    </row>
+    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B66" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E66" s="11">
         <v>11</v>
       </c>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H56" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I56" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="J56" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K56" s="14"/>
-      <c r="L56" s="14"/>
-      <c r="M56" s="14"/>
-      <c r="N56" s="13"/>
-      <c r="O56" s="15">
+      <c r="F66" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" s="11"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K66" s="11"/>
+      <c r="L66" s="11"/>
+      <c r="M66" s="11"/>
+      <c r="N66" s="10"/>
+      <c r="O66" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="7"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="6"/>
-      <c r="K57" s="6"/>
-      <c r="L57" s="6"/>
-      <c r="M57" s="6"/>
-      <c r="N57" s="3"/>
-      <c r="O57" s="8"/>
-    </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E58" s="14">
+    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B67" s="24"/>
+      <c r="C67" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" s="11">
+        <v>25</v>
+      </c>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K67" s="11"/>
+      <c r="L67" s="11"/>
+      <c r="M67" s="11"/>
+      <c r="N67" s="10"/>
+      <c r="O67" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B69" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E69" s="11">
         <v>11</v>
       </c>
-      <c r="F58" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G58" s="14"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K58" s="14"/>
-      <c r="L58" s="14"/>
-      <c r="M58" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="N58" s="13"/>
-      <c r="O58" s="15">
+      <c r="F69" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G69" s="11"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+      <c r="J69" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K69" s="11"/>
+      <c r="L69" s="11"/>
+      <c r="M69" s="11"/>
+      <c r="N69" s="10"/>
+      <c r="O69" s="12">
         <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="12"/>
-      <c r="C59" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E59" s="14">
-        <v>30</v>
-      </c>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K59" s="14"/>
-      <c r="L59" s="14"/>
-      <c r="M59" s="14"/>
-      <c r="N59" s="13"/>
-      <c r="O59" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="12"/>
-      <c r="C60" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="13"/>
-      <c r="I60" s="13"/>
-      <c r="J60" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K60" s="14"/>
-      <c r="L60" s="14"/>
-      <c r="M60" s="14"/>
-      <c r="N60" s="13"/>
-      <c r="O60" s="20">
-        <v>43912</v>
-      </c>
-    </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="12"/>
-      <c r="C61" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D61" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="13"/>
-      <c r="I61" s="13"/>
-      <c r="J61" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K61" s="14"/>
-      <c r="L61" s="14"/>
-      <c r="M61" s="14"/>
-      <c r="N61" s="13"/>
-      <c r="O61" s="21">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="12"/>
-      <c r="C62" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D62" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K62" s="14"/>
-      <c r="L62" s="14"/>
-      <c r="M62" s="14"/>
-      <c r="N62" s="13"/>
-      <c r="O62" s="21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="12"/>
-      <c r="C63" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D63" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E63" s="14">
-        <v>11</v>
-      </c>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H63" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="I63" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="J63" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K63" s="14"/>
-      <c r="L63" s="14"/>
-      <c r="M63" s="14"/>
-      <c r="N63" s="13"/>
-      <c r="O63" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="7"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="6"/>
-      <c r="G64" s="6"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
-      <c r="J64" s="6"/>
-      <c r="K64" s="6"/>
-      <c r="L64" s="6"/>
-      <c r="M64" s="6"/>
-      <c r="N64" s="3"/>
-      <c r="O64" s="8"/>
-    </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B65" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C65" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D65" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E65" s="14">
-        <v>11</v>
-      </c>
-      <c r="F65" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G65" s="14"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K65" s="14"/>
-      <c r="L65" s="14"/>
-      <c r="M65" s="14"/>
-      <c r="N65" s="13"/>
-      <c r="O65" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" s="12"/>
-      <c r="C66" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D66" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E66" s="14">
-        <v>25</v>
-      </c>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="13"/>
-      <c r="I66" s="13"/>
-      <c r="J66" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K66" s="14"/>
-      <c r="L66" s="14"/>
-      <c r="M66" s="14"/>
-      <c r="N66" s="13"/>
-      <c r="O66" s="15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="C68" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="D68" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E68" s="14">
-        <v>11</v>
-      </c>
-      <c r="F68" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G68" s="14"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="13"/>
-      <c r="J68" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K68" s="14"/>
-      <c r="L68" s="14"/>
-      <c r="M68" s="14"/>
-      <c r="N68" s="13"/>
-      <c r="O68" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="19"/>
-      <c r="C69" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D69" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="13"/>
-      <c r="I69" s="13"/>
-      <c r="J69" s="14"/>
-      <c r="K69" s="14"/>
-      <c r="L69" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="M69" s="14"/>
-      <c r="N69" s="13"/>
-      <c r="O69" s="20" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B70" s="19"/>
-      <c r="C70" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D70" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E70" s="14">
-        <v>11</v>
-      </c>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H70" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="I70" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="J70" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K70" s="14"/>
-      <c r="L70" s="14"/>
-      <c r="M70" s="14"/>
-      <c r="N70" s="13"/>
-      <c r="O70" s="15">
-        <v>1</v>
+      <c r="C70" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
+      <c r="J70" s="11"/>
+      <c r="K70" s="11"/>
+      <c r="L70" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="M70" s="11"/>
+      <c r="N70" s="10"/>
+      <c r="O70" s="14" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B71" s="19"/>
-      <c r="C71" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D71" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E71" s="14">
+      <c r="C71" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E71" s="11">
         <v>11</v>
       </c>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H71" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="I71" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="J71" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K71" s="14"/>
-      <c r="L71" s="14"/>
-      <c r="M71" s="14"/>
-      <c r="N71" s="13"/>
-      <c r="O71" s="15">
+      <c r="F71" s="11"/>
+      <c r="G71" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H71" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I71" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="J71" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K71" s="11"/>
+      <c r="L71" s="11"/>
+      <c r="M71" s="11"/>
+      <c r="N71" s="10"/>
+      <c r="O71" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="18"/>
-      <c r="C72" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D72" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E72" s="14">
+      <c r="B72" s="19"/>
+      <c r="C72" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E72" s="11">
         <v>11</v>
       </c>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H72" s="13" t="s">
+      <c r="F72" s="11"/>
+      <c r="G72" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H72" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="I72" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="J72" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K72" s="11"/>
+      <c r="L72" s="11"/>
+      <c r="M72" s="11"/>
+      <c r="N72" s="10"/>
+      <c r="O72" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B73" s="19"/>
+      <c r="C73" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73" s="11">
+        <v>11</v>
+      </c>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H73" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="I72" s="13" t="s">
+      <c r="I73" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J73" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K73" s="11"/>
+      <c r="L73" s="11"/>
+      <c r="M73" s="11"/>
+      <c r="N73" s="10"/>
+      <c r="O73" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B74" s="20"/>
+      <c r="C74" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E74" s="11">
+        <v>11</v>
+      </c>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H74" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="J72" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K72" s="14"/>
-      <c r="L72" s="14"/>
-      <c r="M72" s="14"/>
-      <c r="N72" s="13"/>
-      <c r="O72" s="15">
+      <c r="I74" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J74" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K74" s="11"/>
+      <c r="L74" s="11"/>
+      <c r="M74" s="11"/>
+      <c r="N74" s="10"/>
+      <c r="O74" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="7"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
-      <c r="G73" s="6"/>
-      <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
-      <c r="J73" s="6"/>
-      <c r="K73" s="6"/>
-      <c r="L73" s="6"/>
-      <c r="M73" s="6"/>
-      <c r="N73" s="3"/>
-      <c r="O73" s="8"/>
-    </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="7"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-      <c r="J74" s="6"/>
-      <c r="K74" s="6"/>
-      <c r="L74" s="6"/>
-      <c r="M74" s="6"/>
-      <c r="N74" s="3"/>
-      <c r="O74" s="8"/>
-    </row>
-    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="7"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
-      <c r="G80" s="6"/>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="6"/>
-      <c r="K80" s="6"/>
-      <c r="L80" s="6"/>
-      <c r="M80" s="6"/>
-      <c r="N80" s="3"/>
-      <c r="O80" s="8"/>
-    </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B81" s="7"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
-      <c r="G81" s="6"/>
-      <c r="H81" s="3"/>
-      <c r="I81" s="3"/>
-      <c r="J81" s="6"/>
-      <c r="K81" s="6"/>
-      <c r="L81" s="6"/>
-      <c r="M81" s="6"/>
-      <c r="N81" s="3"/>
-      <c r="O81" s="8"/>
+    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B75" s="7"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="6"/>
+      <c r="L75" s="6"/>
+      <c r="M75" s="6"/>
+      <c r="N75" s="3"/>
+      <c r="O75" s="8"/>
+    </row>
+    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B76" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" s="11">
+        <v>11</v>
+      </c>
+      <c r="F76" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G76" s="11"/>
+      <c r="H76" s="10"/>
+      <c r="I76" s="10"/>
+      <c r="J76" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K76" s="11"/>
+      <c r="L76" s="11"/>
+      <c r="M76" s="11"/>
+      <c r="N76" s="10"/>
+      <c r="O76" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B77" s="24"/>
+      <c r="C77" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E77" s="11">
+        <v>50</v>
+      </c>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="10"/>
+      <c r="I77" s="10"/>
+      <c r="J77" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K77" s="11"/>
+      <c r="L77" s="11"/>
+      <c r="M77" s="11"/>
+      <c r="N77" s="10"/>
+      <c r="O77" s="12" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="82" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B82" s="7"/>
@@ -3630,31 +3734,45 @@
     </row>
     <row r="133" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B133" s="7"/>
+      <c r="C133" s="3"/>
+      <c r="D133" s="3"/>
       <c r="E133" s="6"/>
-      <c r="F133" s="1"/>
-      <c r="G133" s="1"/>
-      <c r="J133" s="1"/>
-      <c r="K133" s="1"/>
-      <c r="L133" s="1"/>
-      <c r="M133" s="1"/>
-      <c r="O133" s="9"/>
+      <c r="F133" s="6"/>
+      <c r="G133" s="6"/>
+      <c r="H133" s="3"/>
+      <c r="I133" s="3"/>
+      <c r="J133" s="6"/>
+      <c r="K133" s="6"/>
+      <c r="L133" s="6"/>
+      <c r="M133" s="6"/>
+      <c r="N133" s="3"/>
+      <c r="O133" s="8"/>
     </row>
     <row r="134" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B134" s="7"/>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
       <c r="E134" s="6"/>
-      <c r="F134" s="1"/>
-      <c r="G134" s="1"/>
-      <c r="J134" s="1"/>
-      <c r="K134" s="1"/>
-      <c r="L134" s="1"/>
-      <c r="M134" s="1"/>
-      <c r="O134" s="9"/>
+      <c r="F134" s="6"/>
+      <c r="G134" s="6"/>
+      <c r="H134" s="3"/>
+      <c r="I134" s="3"/>
+      <c r="J134" s="6"/>
+      <c r="K134" s="6"/>
+      <c r="L134" s="6"/>
+      <c r="M134" s="6"/>
+      <c r="N134" s="3"/>
+      <c r="O134" s="8"/>
     </row>
     <row r="135" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B135" s="7"/>
       <c r="E135" s="6"/>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
+      <c r="J135" s="1"/>
+      <c r="K135" s="1"/>
+      <c r="L135" s="1"/>
+      <c r="M135" s="1"/>
       <c r="O135" s="9"/>
     </row>
     <row r="136" spans="2:15" x14ac:dyDescent="0.25">
@@ -3662,6 +3780,10 @@
       <c r="E136" s="6"/>
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
+      <c r="J136" s="1"/>
+      <c r="K136" s="1"/>
+      <c r="L136" s="1"/>
+      <c r="M136" s="1"/>
       <c r="O136" s="9"/>
     </row>
     <row r="137" spans="2:15" x14ac:dyDescent="0.25">
@@ -3893,12 +4015,14 @@
       <c r="E169" s="6"/>
       <c r="F169" s="1"/>
       <c r="G169" s="1"/>
+      <c r="O169" s="9"/>
     </row>
     <row r="170" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B170" s="7"/>
       <c r="E170" s="6"/>
       <c r="F170" s="1"/>
       <c r="G170" s="1"/>
+      <c r="O170" s="9"/>
     </row>
     <row r="171" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B171" s="7"/>
@@ -3915,10 +4039,14 @@
     <row r="173" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B173" s="7"/>
       <c r="E173" s="6"/>
+      <c r="F173" s="1"/>
+      <c r="G173" s="1"/>
     </row>
     <row r="174" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B174" s="7"/>
       <c r="E174" s="6"/>
+      <c r="F174" s="1"/>
+      <c r="G174" s="1"/>
     </row>
     <row r="175" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B175" s="7"/>
@@ -4248,24 +4376,46 @@
       <c r="B256" s="7"/>
       <c r="E256" s="6"/>
     </row>
-    <row r="257" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B257" s="7"/>
       <c r="E257" s="6"/>
     </row>
-    <row r="258" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B258" s="7"/>
       <c r="E258" s="6"/>
     </row>
-    <row r="259" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E259" s="6"/>
     </row>
+    <row r="260" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E260" s="6"/>
+    </row>
+    <row r="261" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E261" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="B68:B72"/>
+  <mergeCells count="30">
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="B69:B74"/>
     <mergeCell ref="G2:O3"/>
     <mergeCell ref="D2:F3"/>
     <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B51:B56"/>
-    <mergeCell ref="B58:B63"/>
-    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B51:B57"/>
+    <mergeCell ref="B59:B64"/>
+    <mergeCell ref="B66:B67"/>
     <mergeCell ref="B21:B31"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="B36:B37"/>
@@ -4275,19 +4425,6 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B18:B19"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O26" r:id="rId1" xr:uid="{925F1243-137C-438F-85B4-D8DFFF13F326}"/>

</xml_diff>